<commit_message>
- worked a lot - more data prep
</commit_message>
<xml_diff>
--- a/Input Data/Aggregate_Dataset_simple.xlsx
+++ b/Input Data/Aggregate_Dataset_simple.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolaswaser/Desktop/MSA I/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolaswaser/Desktop/MSA I/Data Sets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1949BB4C-E9E3-3147-A15A-4646290C31D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1E0022-920C-544B-A34D-691AF7EDF198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1500" windowWidth="38400" windowHeight="21100" xr2:uid="{BECA30C0-C07E-5143-9059-5C070E5FF597}"/>
+    <workbookView xWindow="48000" yWindow="-1500" windowWidth="19200" windowHeight="21100" xr2:uid="{BECA30C0-C07E-5143-9059-5C070E5FF597}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3745" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3745" uniqueCount="937">
   <si>
     <t>FH</t>
   </si>
@@ -2841,6 +2841,12 @@
   </si>
   <si>
     <t>2015Total</t>
+  </si>
+  <si>
+    <t>V_Dem_Scores</t>
+  </si>
+  <si>
+    <t>FH_Scores</t>
   </si>
 </sst>
 </file>
@@ -3214,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E7045A-3BB1-284B-ABA0-4BC63978FF4E}">
   <dimension ref="A1:DC202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S184" sqref="S184"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="BA1" sqref="BA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3399,7 +3405,7 @@
         <v>871</v>
       </c>
       <c r="AQ1" t="s">
-        <v>852</v>
+        <v>935</v>
       </c>
       <c r="AR1" t="s">
         <v>872</v>
@@ -3429,7 +3435,7 @@
         <v>880</v>
       </c>
       <c r="BA1" t="s">
-        <v>0</v>
+        <v>936</v>
       </c>
       <c r="BB1" t="s">
         <v>929</v>

</xml_diff>

<commit_message>
- v-dem reg finished for now - adjusted data sets several times - started prep for fh
</commit_message>
<xml_diff>
--- a/Input Data/Aggregate_Dataset_simple.xlsx
+++ b/Input Data/Aggregate_Dataset_simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolaswaser/New-project-GitHub-first/R/MSA I/Input Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA9ADC8-0364-DC4A-A92E-D51D0F61E3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0374632C-3A60-1B40-9D82-CD0C85C66829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48220" yWindow="-1500" windowWidth="18980" windowHeight="21100" xr2:uid="{BECA30C0-C07E-5143-9059-5C070E5FF597}"/>
+    <workbookView xWindow="48000" yWindow="-1500" windowWidth="19200" windowHeight="21100" xr2:uid="{BECA30C0-C07E-5143-9059-5C070E5FF597}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3745" uniqueCount="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3745" uniqueCount="935">
   <si>
     <t>FH</t>
   </si>
@@ -2838,6 +2838,9 @@
   </si>
   <si>
     <t>Skopje</t>
+  </si>
+  <si>
+    <t>Rangoon</t>
   </si>
 </sst>
 </file>
@@ -3211,8 +3214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E7045A-3BB1-284B-ABA0-4BC63978FF4E}">
   <dimension ref="A1:DC202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="J133" sqref="J133"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A186" sqref="A186:XFD186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40568,16 +40571,19 @@
         <v>418</v>
       </c>
       <c r="G122">
-        <v>13883</v>
+        <v>678500</v>
+      </c>
+      <c r="H122">
+        <v>309.81950000000001</v>
       </c>
       <c r="I122" t="s">
-        <v>758</v>
+        <v>934</v>
       </c>
       <c r="J122">
-        <v>42.441524000000001</v>
+        <v>16.783329999999999</v>
       </c>
       <c r="K122">
-        <v>19.262108000000001</v>
+        <v>96.166659999999993</v>
       </c>
       <c r="L122">
         <v>0</v>

</xml_diff>